<commit_message>
update done by Samuel Whitby
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ground Segmentation\LiDAR-GS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7987E4E-7370-486B-8F44-549AB0F30848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC44711-61FD-4AAA-9CF2-6F59921EAC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="20832" windowHeight="16656" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="55">
   <si>
     <t>Algorithm Name</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Sum (=1.00)</t>
+  </si>
+  <si>
+    <t>Combined [%]</t>
   </si>
 </sst>
 </file>
@@ -261,7 +264,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -338,11 +341,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -362,14 +378,26 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,16 +705,16 @@
   <dimension ref="A2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -694,7 +722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -702,48 +730,48 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="9">
         <v>0.15</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="9">
         <v>0.4</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="9">
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="9">
         <f>IF(OR(SUM(B6:B9)&gt;1, SUM(B6:B9)&lt;1), "Error!", SUM(B6:B9))</f>
         <v>1</v>
       </c>
@@ -755,31 +783,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="7.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="41" width="8.75" style="1" customWidth="1"/>
-    <col min="42" max="16384" width="8.75" style="1"/>
+    <col min="14" max="41" width="8.69921875" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>3</v>
@@ -818,7 +847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -868,107 +897,107 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="2">
         <f ca="1">IFERROR(E3*pre_weight+F3*rec_weight+G3*iou_weight+(100-H3)*cv_weight, "-")</f>
-        <v>90.795555152982132</v>
+        <v>90.860776838740463</v>
       </c>
       <c r="E3" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>85.96215122430165</v>
+        <v>85.339570161553866</v>
       </c>
       <c r="F3" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!C2:C8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!C9:C12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!C13:C16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!C17:C22")) * 0.25), "-")</f>
-        <v>99.240129311587197</v>
+        <v>96.72901689687329</v>
       </c>
       <c r="G3" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!D2:D8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!D9:D12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!D13:D16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!D17:D22")) * 0.25), "-")</f>
-        <v>86.542859166400078</v>
+        <v>87.955077010562448</v>
       </c>
       <c r="H3" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!E2:E8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!E9:E12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!E13:E16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!E17:E22")) * 0.25), "-")</f>
-        <v>0.99072858195699953</v>
+        <v>0.82749520201986226</v>
       </c>
       <c r="I3" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!F2:F8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!F9:F12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!F13:F16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!F17:F22")) * 0.25), "-")</f>
-        <v>17.01192396313364</v>
+        <v>0.51586981566820278</v>
       </c>
       <c r="J3" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!G2:G8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!G9:G12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!G13:G16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!G17:G22")) * 0.25), "-")</f>
-        <v>-4.5122887864826539E-4</v>
+        <v>1.6474654377880125E-2</v>
       </c>
       <c r="K3" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!H2:H8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!H9:H12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!H13:H16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!H17:H22")) * 0.25), "-")</f>
-        <v>0.13008832565284179</v>
+        <v>0.13277649769585251</v>
       </c>
       <c r="L3" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>85.96215122430165</v>
+        <v>85.339570161553866</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="2">
         <f ca="1">IFERROR(E4*pre_weight+F4*rec_weight+G4*iou_weight+(100-H4)*cv_weight, "-")</f>
-        <v>90.860776838740463</v>
+        <v>90.795555152982132</v>
       </c>
       <c r="E4" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>85.339570161553866</v>
+        <v>85.96215122430165</v>
       </c>
       <c r="F4" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C2:C8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C9:C12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C13:C16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C17:C22")) * 0.25), "-")</f>
-        <v>96.72901689687329</v>
+        <v>99.240129311587197</v>
       </c>
       <c r="G4" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D2:D8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D9:D12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D13:D16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D17:D22")) * 0.25), "-")</f>
-        <v>87.955077010562448</v>
+        <v>86.542859166400078</v>
       </c>
       <c r="H4" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E2:E8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E9:E12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E13:E16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E17:E22")) * 0.25), "-")</f>
-        <v>0.82749520201986226</v>
+        <v>0.99072858195699953</v>
       </c>
       <c r="I4" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F2:F8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F9:F12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F13:F16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F17:F22")) * 0.25), "-")</f>
-        <v>0.51586981566820278</v>
+        <v>17.01192396313364</v>
       </c>
       <c r="J4" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G2:G8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G9:G12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G13:G16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G17:G22")) * 0.25), "-")</f>
-        <v>1.6474654377880125E-2</v>
+        <v>-4.5122887864826539E-4</v>
       </c>
       <c r="K4" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H2:H8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H9:H12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H13:H16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H17:H22")) * 0.25), "-")</f>
-        <v>0.13277649769585251</v>
+        <v>0.13008832565284179</v>
       </c>
       <c r="L4" s="2">
         <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>85.339570161553866</v>
+        <v>85.96215122430165</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1018,7 +1047,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1067,12 +1096,12 @@
         <v>-</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1081,558 +1110,593 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="41" width="8.75" style="1" customWidth="1"/>
-    <col min="42" max="16384" width="8.75" style="1"/>
+    <col min="1" max="1" width="1.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="42" width="8.69921875" style="1" customWidth="1"/>
+    <col min="43" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="14">
+        <f ca="1">IFERROR(AVERAGE(E2:E3),"-")</f>
+        <v>90.730086574554477</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2">
-        <f ca="1">IFERROR(E2*pre_weight+F2*rec_weight+G2*iou_weight+(100-H2)*cv_weight, "-")</f>
+      <c r="E2" s="2">
+        <f t="shared" ref="E2:E3" ca="1" si="0">IFERROR(F2*pre_weight+G2*rec_weight+H2*iou_weight+(100-I2)*cv_weight, "-")</f>
         <v>91.685283332814535</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B9:B12")), "-")</f>
         <v>87.132520116457528</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C9:C12")), "-")</f>
         <v>98.234119676471366</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D9:D12")), "-")</f>
         <v>88.464006043726442</v>
       </c>
-      <c r="H2" s="2">
+      <c r="I2" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E9:E12")), "-")</f>
         <v>1.0928353263056589</v>
       </c>
-      <c r="I2" s="2">
+      <c r="J2" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F9:F12")), "-")</f>
         <v>0.3564516129032258</v>
       </c>
-      <c r="J2" s="2">
+      <c r="K2" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G9:G12")), "-")</f>
         <v>-8.0645161290322299E-4</v>
       </c>
-      <c r="K2" s="2">
+      <c r="L2" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H9:H12")), "-")</f>
         <v>1.6129032258064516E-2</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!I9:I12")), "-")</f>
         <v>61.783431432306124</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="2">
-        <f ca="1">IFERROR(E3*pre_weight+F3*rec_weight+G3*iou_weight+(100-H3)*cv_weight, "-")</f>
+      <c r="E3" s="2">
+        <f t="shared" ca="1" si="0"/>
         <v>89.774889816294419</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B2:B8")), "-")</f>
         <v>84.182073809950879</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C2:C8")), "-")</f>
         <v>98.631698999892038</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D2:D8")), "-")</f>
         <v>85.305095307992445</v>
       </c>
-      <c r="H3" s="2">
+      <c r="I3" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E2:E8")), "-")</f>
         <v>0.93710804687043348</v>
       </c>
-      <c r="I3" s="2">
+      <c r="J3" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F2:F8")), "-")</f>
         <v>0.20691244239631335</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G2:G8")), "-")</f>
         <v>-4.6082949308755598E-4</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H2:H8")), "-")</f>
         <v>7.3732718894009244E-2</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!I2:I8")), "-")</f>
         <v>94.301250454196307</v>
       </c>
-      <c r="M3" s="10"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="N3" s="11"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="16">
+        <f t="shared" ref="C4:C11" ca="1" si="1">IFERROR(AVERAGE(E4:E5),"-")</f>
+        <v>90.009220641129318</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="2">
-        <f ca="1">IFERROR(E4*pre_weight+F4*rec_weight+G4*iou_weight+(100-H4)*cv_weight, "-")</f>
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E11" ca="1" si="2">IFERROR(F4*pre_weight+G4*rec_weight+H4*iou_weight+(100-I4)*cv_weight, "-")</f>
         <v>89.84015336241643</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B9:B12")), "-")</f>
         <v>84.481247839053438</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C9:C12")), "-")</f>
         <v>97.972552258545278</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D9:D12")), "-")</f>
         <v>85.984504763608982</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E9:E12")), "-")</f>
         <v>1.8492167078616293</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F9:F12")), "-")</f>
         <v>18.671774193548384</v>
       </c>
-      <c r="J4" s="2">
+      <c r="K4" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G9:G12")), "-")</f>
         <v>8.8709677419356089E-3</v>
       </c>
-      <c r="K4" s="2">
+      <c r="L4" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H9:H12")), "-")</f>
         <v>-1.6129032258064516E-2</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!I9:I12")), "-")</f>
         <v>32.745342136067734</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N4" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="1" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="2">
-        <f ca="1">IFERROR(E5*pre_weight+F5*rec_weight+G5*iou_weight+(100-H5)*cv_weight, "-")</f>
+      <c r="E5" s="2">
+        <f t="shared" ca="1" si="2"/>
         <v>90.178287919842205</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B2:B8")), "-")</f>
         <v>85.273989895297632</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C2:C8")), "-")</f>
         <v>99.007174878695011</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D2:D8")), "-")</f>
         <v>86.078634345517045</v>
       </c>
-      <c r="H5" s="2">
+      <c r="I5" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E2:E8")), "-")</f>
         <v>2.1136976199663691</v>
       </c>
-      <c r="I5" s="2">
+      <c r="J5" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F2:F8")), "-")</f>
         <v>15.500921658986174</v>
       </c>
-      <c r="J5" s="2">
+      <c r="K5" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G2:G8")), "-")</f>
         <v>5.9907834101382285E-3</v>
       </c>
-      <c r="K5" s="2">
+      <c r="L5" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H2:H8")), "-")</f>
         <v>0.11981566820276499</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!I2:I8")), "-")</f>
         <v>32.550679183483389</v>
       </c>
-      <c r="M5" s="10"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
+      <c r="N5" s="11"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="16">
+        <f t="shared" ref="C6:C11" ca="1" si="3">IFERROR(AVERAGE(E6:E7),"-")</f>
+        <v>89.91692889208457</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="2">
-        <f ca="1">IFERROR(E6*pre_weight+F6*rec_weight+G6*iou_weight+(100-H6)*cv_weight, "-")</f>
+      <c r="E6" s="2">
+        <f t="shared" ca="1" si="2"/>
         <v>90.997344870744158</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B9:B12")), "-")</f>
         <v>86.140953438629055</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C9:C12")), "-")</f>
         <v>96.690725352351294</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D9:D12")), "-")</f>
         <v>88.400411526222427</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E9:E12")), "-")</f>
         <v>2.0083345112738544</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F9:F12")), "-")</f>
         <v>1.075</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G9:G12")), "-")</f>
         <v>4.8387096774193377E-3</v>
       </c>
-      <c r="K6" s="2">
+      <c r="L6" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H9:H12")), "-")</f>
         <v>0.44354838709677424</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!I9:I12")), "-")</f>
         <v>97.730375137526224</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="N6" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="1" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2">
-        <f ca="1">IFERROR(E7*pre_weight+F7*rec_weight+G7*iou_weight+(100-H7)*cv_weight, "-")</f>
+      <c r="E7" s="2">
+        <f t="shared" ca="1" si="2"/>
         <v>88.836512913424983</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B2:B8")), "-")</f>
         <v>81.316494372279379</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C2:C8")), "-")</f>
         <v>93.352206739636287</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D2:D8")), "-")</f>
         <v>86.912218921927007</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E2:E8")), "-")</f>
         <v>1.3016462968055944</v>
       </c>
-      <c r="I7" s="2">
+      <c r="J7" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F2:F8")), "-")</f>
         <v>0.58847926267281114</v>
       </c>
-      <c r="J7" s="2">
+      <c r="K7" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G2:G8")), "-")</f>
         <v>1.1059907834101343E-2</v>
       </c>
-      <c r="K7" s="2">
+      <c r="L7" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H2:H8")), "-")</f>
         <v>8.7557603686635968E-2</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!I2:I8")), "-")</f>
         <v>92.681978262844083</v>
       </c>
-      <c r="M7" s="10"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="16">
+        <f t="shared" ref="C8:C11" ca="1" si="4">IFERROR(AVERAGE(E8:E9),"-")</f>
+        <v>69.576028661651776</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="2">
-        <f ca="1">IFERROR(E8*pre_weight+F8*rec_weight+G8*iou_weight+(100-H8)*cv_weight, "-")</f>
+      <c r="E8" s="2">
+        <f t="shared" ca="1" si="2"/>
         <v>93.549025090524992</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!B9:B12")), "-")</f>
         <v>86.019075229999999</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!C9:C12")), "-")</f>
         <v>86.700224882500009</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!D9:D12")), "-")</f>
         <v>99.187658499999998</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!E9:E12")), "-")</f>
         <v>3.1792042467499999</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!F9:F12")), "-")</f>
         <v>0.78790322575000005</v>
       </c>
-      <c r="J8" s="2">
+      <c r="K8" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!G9:G12")), "-")</f>
         <v>-8.0645162500000006E-3</v>
       </c>
-      <c r="K8" s="2">
+      <c r="L8" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!H9:H12")), "-")</f>
         <v>0.32258064525000002</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!I9:I12")), "-")</f>
         <v>25.983034595000003</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="N8" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="1" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="2">
-        <f ca="1">IFERROR(E9*pre_weight+F9*rec_weight+G9*iou_weight+(100-H9)*cv_weight, "-")</f>
+      <c r="E9" s="2">
+        <f t="shared" ca="1" si="2"/>
         <v>45.603032232778574</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!B2:B8")), "-")</f>
         <v>29.187782790142858</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!C2:C8")), "-")</f>
         <v>95.973811007142857</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!D2:D8")), "-")</f>
         <v>29.626548686285712</v>
       </c>
-      <c r="H9" s="2">
+      <c r="I9" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!E2:E8")), "-")</f>
         <v>39.703022951714289</v>
       </c>
-      <c r="I9" s="2">
+      <c r="J9" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!F2:F8")), "-")</f>
         <v>0.67695852542857149</v>
       </c>
-      <c r="J9" s="2">
+      <c r="K9" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!G2:G8")), "-")</f>
         <v>-1.0138248857142857E-2</v>
       </c>
-      <c r="K9" s="2">
+      <c r="L9" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!H2:H8")), "-")</f>
         <v>-0.83870967728571444</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!I2:I8")), "-")</f>
         <v>54.900533042857148</v>
       </c>
-      <c r="M9" s="10"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
         <v>5</v>
       </c>
-      <c r="B10" s="9" t="str">
+      <c r="B10" s="12" t="str">
         <f>algorithm_name</f>
         <v>-</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="16" t="str">
+        <f t="shared" ref="C10:C11" ca="1" si="5">IFERROR(AVERAGE(E10:E11),"-")</f>
+        <v>-</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="2" t="str">
-        <f ca="1">IFERROR(E10*pre_weight+F10*rec_weight+G10*iou_weight+(100-H10)*cv_weight, "-")</f>
-        <v>-</v>
-      </c>
       <c r="E10" s="2" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F10" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!B9:B12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="F10" s="2" t="str">
+      <c r="G10" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!C9:C12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="G10" s="2" t="str">
+      <c r="H10" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!D9:D12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="H10" s="2" t="str">
+      <c r="I10" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!E9:E12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="I10" s="2" t="str">
+      <c r="J10" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!F9:F12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="J10" s="2" t="str">
+      <c r="K10" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!G9:G12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="K10" s="2" t="str">
+      <c r="L10" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!H9:H12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="L10" s="2" t="str">
+      <c r="M10" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!I9:I12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="M10" s="9" t="str">
+      <c r="N10" s="12" t="str">
         <f>system</f>
         <v>-</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="1" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="2" t="str">
-        <f ca="1">IFERROR(E11*pre_weight+F11*rec_weight+G11*iou_weight+(100-H11)*cv_weight, "-")</f>
-        <v>-</v>
-      </c>
       <c r="E11" s="2" t="str">
+        <f t="shared" ca="1" si="2"/>
+        <v>-</v>
+      </c>
+      <c r="F11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!B2:B8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="F11" s="2" t="str">
+      <c r="G11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!C2:C8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="G11" s="2" t="str">
+      <c r="H11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!D2:D8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="H11" s="2" t="str">
+      <c r="I11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!E2:E8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="I11" s="2" t="str">
+      <c r="J11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!F2:F8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="J11" s="2" t="str">
+      <c r="K11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!G2:G8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="K11" s="2" t="str">
+      <c r="L11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!H2:H8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="L11" s="2" t="str">
+      <c r="M11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!I2:I8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="M11" s="10"/>
+      <c r="N11" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="M2:M3"/>
+  <mergeCells count="20">
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="N2:N3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N10:N11"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="N6:N7"/>
     <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1640,558 +1704,593 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="6.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="33" width="8.75" style="1" customWidth="1"/>
-    <col min="34" max="16384" width="8.75" style="1"/>
+    <col min="1" max="1" width="1.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="33" width="8.69921875" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="11">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="14">
+        <f ca="1">IFERROR(AVERAGE(E2:E3),"-")</f>
+        <v>92.820362579958342</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2">
+        <f t="shared" ref="E2:E9" ca="1" si="0">IFERROR(F2*pre_weight+G2*rec_weight+H2*iou_weight+(100-I2)*cv_weight, "-")</f>
+        <v>99.304945170916682</v>
+      </c>
+      <c r="F2" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B17:B22")), "-")</f>
+        <v>98.930684878333338</v>
+      </c>
+      <c r="G2" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C17:C22")), "-")</f>
+        <v>100</v>
+      </c>
+      <c r="H2" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D17:D22")), "-")</f>
+        <v>98.930684878333338</v>
+      </c>
+      <c r="I2" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E17:E22")), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F17:F22")), "-")</f>
+        <v>1.5833333333333333</v>
+      </c>
+      <c r="K2" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G17:G22")), "-")</f>
+        <v>-1.6666666666666666E-2</v>
+      </c>
+      <c r="L2" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H17:H22")), "-")</f>
+        <v>8</v>
+      </c>
+      <c r="M2" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!I17:I22")), "-")</f>
+        <v>19.377807274999999</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>86.335779989000002</v>
+      </c>
+      <c r="F3" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B13:B16")), "-")</f>
+        <v>78.978123060000001</v>
+      </c>
+      <c r="G3" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C13:C16")), "-")</f>
+        <v>100</v>
+      </c>
+      <c r="H3" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D13:D16")), "-")</f>
+        <v>78.978123060000001</v>
+      </c>
+      <c r="I3" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E13:E16")), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F13:F16")), "-")</f>
+        <v>1.375</v>
+      </c>
+      <c r="K3" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G13:G16")), "-")</f>
+        <v>-2.5000000000000001E-2</v>
+      </c>
+      <c r="L3" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H13:H16")), "-")</f>
+        <v>-3.25</v>
+      </c>
+      <c r="M3" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!I13:I16")), "-")</f>
+        <v>18.368882567500002</v>
+      </c>
+      <c r="N3" s="11"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="16">
+        <f t="shared" ref="C4:C11" ca="1" si="1">IFERROR(AVERAGE(E4:E5),"-")</f>
+        <v>91.804624785396385</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>93.412023331820023</v>
+      </c>
+      <c r="F4" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B17:B22")), "-")</f>
+        <v>89.163734620541391</v>
+      </c>
+      <c r="G4" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C17:C22")), "-")</f>
+        <v>97.628049265160499</v>
+      </c>
+      <c r="H4" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D17:D22")), "-")</f>
+        <v>91.19220571727648</v>
+      </c>
+      <c r="I4" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E17:E22")), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F17:F22")), "-")</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="K4" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G17:G22")), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H17:H22")), "-")</f>
+        <v>-0.50000000000000011</v>
+      </c>
+      <c r="M4" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!I17:I22")), "-")</f>
+        <v>146.35557969909368</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" ca="1" si="0"/>
+        <v>90.197226238972732</v>
+      </c>
+      <c r="F5" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B13:B16")), "-")</f>
+        <v>84.737098214765638</v>
+      </c>
+      <c r="G5" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C13:C16")), "-")</f>
+        <v>99.245086230345109</v>
+      </c>
+      <c r="H5" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D13:D16")), "-")</f>
+        <v>85.315471876823878</v>
+      </c>
+      <c r="I5" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E13:E16")), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F13:F16")), "-")</f>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="K5" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G13:G16")), "-")</f>
+        <v>4.9999999999999822E-2</v>
+      </c>
+      <c r="L5" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H13:H16")), "-")</f>
+        <v>0.5</v>
+      </c>
+      <c r="M5" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!I13:I16")), "-")</f>
+        <v>96.245946276680598</v>
+      </c>
+      <c r="N5" s="11"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
+        <v>3</v>
+      </c>
+      <c r="B6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C6" s="16">
+        <f t="shared" ref="C6:C11" ca="1" si="2">IFERROR(AVERAGE(E6:E7),"-")</f>
+        <v>91.581889664834932</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2">
-        <f ca="1">IFERROR(E2*pre_weight+F2*rec_weight+G2*iou_weight+(100-H2)*cv_weight, "-")</f>
+      <c r="E6" s="2">
+        <f t="shared" ca="1" si="0"/>
         <v>93.877317485517025</v>
       </c>
-      <c r="E2" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B17:B22")), "-")</f>
+      <c r="F6" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B17:B22")), "-")</f>
         <v>90.577744542562314</v>
       </c>
-      <c r="F2" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C17:C22")), "-")</f>
+      <c r="G6" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C17:C22")), "-")</f>
         <v>99.989442673142193</v>
       </c>
-      <c r="G2" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D17:D22")), "-")</f>
+      <c r="H6" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D17:D22")), "-")</f>
         <v>90.586162372262791</v>
       </c>
-      <c r="H2" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E17:E22")), "-")</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F17:F22")), "-")</f>
+      <c r="I6" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E17:E22")), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F17:F22")), "-")</f>
         <v>15.4</v>
       </c>
-      <c r="J2" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G17:G22")), "-")</f>
+      <c r="K6" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G17:G22")), "-")</f>
         <v>-1.6666666666666899E-2</v>
       </c>
-      <c r="K2" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H17:H22")), "-")</f>
+      <c r="L6" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H17:H22")), "-")</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="L2" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!I17:I22")), "-")</f>
+      <c r="M6" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!I17:I22")), "-")</f>
         <v>48.746001630501063</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N6" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="1" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="2">
-        <f ca="1">IFERROR(E3*pre_weight+F3*rec_weight+G3*iou_weight+(100-H3)*cv_weight, "-")</f>
+      <c r="E7" s="2">
+        <f t="shared" ca="1" si="0"/>
         <v>89.286461844152839</v>
       </c>
-      <c r="E3" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B13:B16")), "-")</f>
+      <c r="F7" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B13:B16")), "-")</f>
         <v>83.515622620293229</v>
       </c>
-      <c r="F3" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C13:C16")), "-")</f>
+      <c r="G7" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C13:C16")), "-")</f>
         <v>99.991347435966304</v>
       </c>
-      <c r="G3" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D13:D16")), "-")</f>
+      <c r="H7" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D13:D16")), "-")</f>
         <v>83.522135184211464</v>
       </c>
-      <c r="H3" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E13:E16")), "-")</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F13:F16")), "-")</f>
+      <c r="I7" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E13:E16")), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F13:F16")), "-")</f>
         <v>18.475000000000001</v>
       </c>
-      <c r="J3" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G13:G16")), "-")</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H13:H16")), "-")</f>
+      <c r="K7" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G13:G16")), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H13:H16")), "-")</f>
         <v>0.25</v>
       </c>
-      <c r="L3" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!I13:I16")), "-")</f>
+      <c r="M7" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!I13:I16")), "-")</f>
         <v>29.583004715014212</v>
       </c>
-      <c r="M3" s="10"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="12">
+        <v>4</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C8" s="16">
+        <f t="shared" ref="C8:C11" ca="1" si="3">IFERROR(AVERAGE(E8:E9),"-")</f>
+        <v>91.170415627775355</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="2">
-        <f ca="1">IFERROR(E4*pre_weight+F4*rec_weight+G4*iou_weight+(100-H4)*cv_weight, "-")</f>
+      <c r="E8" s="2">
+        <f t="shared" ca="1" si="0"/>
         <v>92.616228914278651</v>
       </c>
-      <c r="E4" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B17:B22")), "-")</f>
+      <c r="F8" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!B17:B22")), "-")</f>
         <v>88.111774280571254</v>
       </c>
-      <c r="F4" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C17:C22")), "-")</f>
+      <c r="G8" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!C17:C22")), "-")</f>
         <v>97.877081461267494</v>
       </c>
-      <c r="G4" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D17:D22")), "-")</f>
+      <c r="H8" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!D17:D22")), "-")</f>
         <v>89.766807812364291</v>
       </c>
-      <c r="H4" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E17:E22")), "-")</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F17:F22")), "-")</f>
+      <c r="I8" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!E17:E22")), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!F17:F22")), "-")</f>
         <v>0.38333333333333336</v>
       </c>
-      <c r="J4" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G17:G22")), "-")</f>
+      <c r="K8" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!G17:G22")), "-")</f>
         <v>1.6666666666666607E-2</v>
       </c>
-      <c r="K4" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H17:H22")), "-")</f>
+      <c r="L8" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!H17:H22")), "-")</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="L4" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!I17:I22")), "-")</f>
+      <c r="M8" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!I17:I22")), "-")</f>
         <v>108.2016928782039</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="N8" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="1" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="2">
-        <f ca="1">IFERROR(E5*pre_weight+F5*rec_weight+G5*iou_weight+(100-H5)*cv_weight, "-")</f>
+      <c r="E9" s="2">
+        <f t="shared" ca="1" si="0"/>
         <v>89.72460234127206</v>
       </c>
-      <c r="E5" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B13:B16")), "-")</f>
+      <c r="F9" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!B13:B16")), "-")</f>
         <v>81.77780447730558</v>
       </c>
-      <c r="F5" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C13:C16")), "-")</f>
+      <c r="G9" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!C13:C16")), "-")</f>
         <v>91.359332012837541</v>
       </c>
-      <c r="G5" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D13:D16")), "-")</f>
+      <c r="H9" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!D13:D16")), "-")</f>
         <v>88.940628550050064</v>
       </c>
-      <c r="H5" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E13:E16")), "-")</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F13:F16")), "-")</f>
+      <c r="I9" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!E13:E16")), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!F13:F16")), "-")</f>
         <v>0.25</v>
       </c>
-      <c r="J5" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G13:G16")), "-")</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H13:H16")), "-")</f>
+      <c r="K9" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!G13:G16")), "-")</f>
+        <v>0</v>
+      </c>
+      <c r="L9" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!H13:H16")), "-")</f>
         <v>0.25</v>
       </c>
-      <c r="L5" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!I13:I16")), "-")</f>
+      <c r="M9" s="2">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!I13:I16")), "-")</f>
         <v>62.89510744849359</v>
       </c>
-      <c r="M5" s="10"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="9">
-        <v>3</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="12">
+        <v>5</v>
+      </c>
+      <c r="B10" s="12" t="str">
+        <f>algorithm_name</f>
+        <v>-</v>
+      </c>
+      <c r="C10" s="16" t="str">
+        <f t="shared" ref="C10:C11" ca="1" si="4">IFERROR(AVERAGE(E10:E11),"-")</f>
+        <v>-</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2">
-        <f ca="1">IFERROR(E6*pre_weight+F6*rec_weight+G6*iou_weight+(100-H6)*cv_weight, "-")</f>
-        <v>93.412023331820023</v>
-      </c>
-      <c r="E6" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B17:B22")), "-")</f>
-        <v>89.163734620541391</v>
-      </c>
-      <c r="F6" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C17:C22")), "-")</f>
-        <v>97.628049265160499</v>
-      </c>
-      <c r="G6" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D17:D22")), "-")</f>
-        <v>91.19220571727648</v>
-      </c>
-      <c r="H6" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E17:E22")), "-")</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F17:F22")), "-")</f>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="J6" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G17:G22")), "-")</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H17:H22")), "-")</f>
-        <v>-0.50000000000000011</v>
-      </c>
-      <c r="L6" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!I17:I22")), "-")</f>
-        <v>146.35557969909368</v>
-      </c>
-      <c r="M6" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="1" t="s">
+      <c r="E10" s="2" t="str">
+        <f t="shared" ref="E10:E11" ca="1" si="5">IFERROR(F10*pre_weight+G10*rec_weight+H10*iou_weight+(100-I10)*cv_weight, "-")</f>
+        <v>-</v>
+      </c>
+      <c r="F10" s="2" t="str">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!B17:B22")), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="G10" s="2" t="str">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!C17:C22")), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="H10" s="2" t="str">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!D17:D22")), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="I10" s="2" t="str">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!E17:E22")), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="J10" s="2" t="str">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!F17:F22")), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="K10" s="2" t="str">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!G17:G22")), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="L10" s="2" t="str">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!H17:H22")), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="M10" s="2" t="str">
+        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!I17:I22")), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="N10" s="12" t="str">
+        <f>system</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="2">
-        <f ca="1">IFERROR(E7*pre_weight+F7*rec_weight+G7*iou_weight+(100-H7)*cv_weight, "-")</f>
-        <v>90.197226238972732</v>
-      </c>
-      <c r="E7" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B13:B16")), "-")</f>
-        <v>84.737098214765638</v>
-      </c>
-      <c r="F7" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C13:C16")), "-")</f>
-        <v>99.245086230345109</v>
-      </c>
-      <c r="G7" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D13:D16")), "-")</f>
-        <v>85.315471876823878</v>
-      </c>
-      <c r="H7" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E13:E16")), "-")</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F13:F16")), "-")</f>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="J7" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G13:G16")), "-")</f>
-        <v>4.9999999999999822E-2</v>
-      </c>
-      <c r="K7" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H13:H16")), "-")</f>
-        <v>0.5</v>
-      </c>
-      <c r="L7" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!I13:I16")), "-")</f>
-        <v>96.245946276680598</v>
-      </c>
-      <c r="M7" s="10"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="9">
-        <v>4</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="2">
-        <f ca="1">IFERROR(E8*pre_weight+F8*rec_weight+G8*iou_weight+(100-H8)*cv_weight, "-")</f>
-        <v>99.304945170916682</v>
-      </c>
-      <c r="E8" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!B17:B22")), "-")</f>
-        <v>98.930684878333338</v>
-      </c>
-      <c r="F8" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!C17:C22")), "-")</f>
-        <v>100</v>
-      </c>
-      <c r="G8" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!D17:D22")), "-")</f>
-        <v>98.930684878333338</v>
-      </c>
-      <c r="H8" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!E17:E22")), "-")</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!F17:F22")), "-")</f>
-        <v>1.5833333333333333</v>
-      </c>
-      <c r="J8" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!G17:G22")), "-")</f>
-        <v>-1.6666666666666666E-2</v>
-      </c>
-      <c r="K8" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!H17:H22")), "-")</f>
-        <v>8</v>
-      </c>
-      <c r="L8" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!I17:I22")), "-")</f>
-        <v>19.377807274999999</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="2">
-        <f ca="1">IFERROR(E9*pre_weight+F9*rec_weight+G9*iou_weight+(100-H9)*cv_weight, "-")</f>
-        <v>86.335779989000002</v>
-      </c>
-      <c r="E9" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!B13:B16")), "-")</f>
-        <v>78.978123060000001</v>
-      </c>
-      <c r="F9" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!C13:C16")), "-")</f>
-        <v>100</v>
-      </c>
-      <c r="G9" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!D13:D16")), "-")</f>
-        <v>78.978123060000001</v>
-      </c>
-      <c r="H9" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!E13:E16")), "-")</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!F13:F16")), "-")</f>
-        <v>1.375</v>
-      </c>
-      <c r="J9" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!G13:G16")), "-")</f>
-        <v>-2.5000000000000001E-2</v>
-      </c>
-      <c r="K9" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!H13:H16")), "-")</f>
-        <v>-3.25</v>
-      </c>
-      <c r="L9" s="2">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!I13:I16")), "-")</f>
-        <v>18.368882567500002</v>
-      </c>
-      <c r="M9" s="10"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>5</v>
-      </c>
-      <c r="B10" s="9" t="str">
-        <f>algorithm_name</f>
-        <v>-</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2" t="str">
-        <f ca="1">IFERROR(E10*pre_weight+F10*rec_weight+G10*iou_weight+(100-H10)*cv_weight, "-")</f>
-        <v>-</v>
-      </c>
-      <c r="E10" s="2" t="str">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!B17:B22")), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="F10" s="2" t="str">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!C17:C22")), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="G10" s="2" t="str">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!D17:D22")), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="H10" s="2" t="str">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!E17:E22")), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="I10" s="2" t="str">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!F17:F22")), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="J10" s="2" t="str">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!G17:G22")), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="K10" s="2" t="str">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!H17:H22")), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="L10" s="2" t="str">
-        <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!I17:I22")), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="M10" s="9" t="str">
-        <f>system</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="2" t="str">
-        <f ca="1">IFERROR(E11*pre_weight+F11*rec_weight+G11*iou_weight+(100-H11)*cv_weight, "-")</f>
-        <v>-</v>
-      </c>
       <c r="E11" s="2" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!B13:B16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="F11" s="2" t="str">
+      <c r="G11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!C13:C16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="G11" s="2" t="str">
+      <c r="H11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!D13:D16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="H11" s="2" t="str">
+      <c r="I11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!E13:E16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="I11" s="2" t="str">
+      <c r="J11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!F13:F16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="J11" s="2" t="str">
+      <c r="K11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!G13:G16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="K11" s="2" t="str">
+      <c r="L11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!H13:H16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="L11" s="2" t="str">
+      <c r="M11" s="2" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!I13:I16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="M11" s="10"/>
+      <c r="N11" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="B2:B3"/>
+  <mergeCells count="20">
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="N10:N11"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2205,21 +2304,21 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.8984375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.09765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.3984375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="9" style="2" customWidth="1"/>
     <col min="13" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>26</v>
       </c>
@@ -2248,7 +2347,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -2277,7 +2376,7 @@
         <v>92.728687654757692</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -2306,7 +2405,7 @@
         <v>92.489448499415644</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -2335,7 +2434,7 @@
         <v>123.7111845210005</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -2364,7 +2463,7 @@
         <v>74.28937813280433</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -2393,7 +2492,7 @@
         <v>94.355799514082605</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -2422,7 +2521,7 @@
         <v>102.0015564202335</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -2451,7 +2550,7 @@
         <v>80.532698437079986</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -2480,7 +2579,7 @@
         <v>59.466681789825891</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -2509,7 +2608,7 @@
         <v>60.49593261408873</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -2538,7 +2637,7 @@
         <v>68.588173731030878</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
@@ -2567,7 +2666,7 @@
         <v>58.582937594279009</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -2596,7 +2695,7 @@
         <v>67.572682895393982</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -2625,7 +2724,7 @@
         <v>61.631998119140682</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -2654,7 +2753,7 @@
         <v>61.234291053492171</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -2683,7 +2782,7 @@
         <v>61.141457725947532</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>42</v>
       </c>
@@ -2712,7 +2811,7 @@
         <v>71.335340238447543</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
@@ -2741,7 +2840,7 @@
         <v>104.3826589019959</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -2770,7 +2869,7 @@
         <v>39.466516113855562</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
@@ -2799,7 +2898,7 @@
         <v>266.15292848530999</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
@@ -2828,7 +2927,7 @@
         <v>107.8365856793932</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
@@ -2870,21 +2969,21 @@
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.8984375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.09765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.3984375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="19" width="9" style="2" customWidth="1"/>
     <col min="20" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>26</v>
       </c>
@@ -2913,7 +3012,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -2942,7 +3041,7 @@
         <v>90.406173212053289</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -2971,7 +3070,7 @@
         <v>90.060637292793956</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -3000,7 +3099,7 @@
         <v>106.83675080873179</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -3029,7 +3128,7 @@
         <v>90.470524794547146</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -3058,7 +3157,7 @@
         <v>86.206766144612985</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -3087,7 +3186,7 @@
         <v>90.615161924514439</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -3116,7 +3215,7 @@
         <v>94.177833662654933</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -3145,7 +3244,7 @@
         <v>101.23588617218989</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -3174,7 +3273,7 @@
         <v>96.08943871706758</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -3203,7 +3302,7 @@
         <v>100.41426861383771</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
@@ -3232,7 +3331,7 @@
         <v>93.181907047009688</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -3261,7 +3360,7 @@
         <v>96.752185647389908</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -3290,7 +3389,7 @@
         <v>98.430113583028259</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -3319,7 +3418,7 @@
         <v>92.771759085178388</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -3348,7 +3447,7 @@
         <v>97.02972679112591</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>42</v>
       </c>
@@ -3377,7 +3476,7 @@
         <v>108.9005322601584</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
@@ -3406,7 +3505,7 @@
         <v>120.31162870747519</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -3435,7 +3534,7 @@
         <v>62.585672292104988</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
@@ -3464,7 +3563,7 @@
         <v>324.13477588871717</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
@@ -3493,7 +3592,7 @@
         <v>166.42082291790661</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
@@ -3535,21 +3634,21 @@
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.8984375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.09765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.3984375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9" style="2" customWidth="1"/>
     <col min="12" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
@@ -3578,7 +3677,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -3607,7 +3706,7 @@
         <v>36.590252030463503</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -3636,7 +3735,7 @@
         <v>31.936405929964291</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -3665,7 +3764,7 @@
         <v>38.420988027517467</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -3694,7 +3793,7 @@
         <v>29.541512889139319</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -3723,7 +3822,7 @@
         <v>27.916987260552979</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -3752,7 +3851,7 @@
         <v>31.588133844450638</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -3781,7 +3880,7 @@
         <v>31.86047430229555</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -3810,7 +3909,7 @@
         <v>30.23248639492558</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -3839,7 +3938,7 @@
         <v>32.700045218530242</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -3868,7 +3967,7 @@
         <v>34.395329003477009</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
@@ -3897,7 +3996,7 @@
         <v>33.653507927338083</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -3926,7 +4025,7 @@
         <v>25.897319692020819</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -3955,7 +4054,7 @@
         <v>28.56104702629823</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -3984,7 +4083,7 @@
         <v>32.798748827025342</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -4013,7 +4112,7 @@
         <v>31.074903314712461</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>42</v>
       </c>
@@ -4042,7 +4141,7 @@
         <v>35.982224662423008</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
@@ -4071,7 +4170,7 @@
         <v>55.346968937214641</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -4100,7 +4199,7 @@
         <v>24.998235827015691</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
@@ -4129,7 +4228,7 @@
         <v>91.670761026358349</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
@@ -4158,7 +4257,7 @@
         <v>54.593429478835837</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
@@ -4196,25 +4295,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.3984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.19921875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.8984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.8984375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.09765625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.3984375" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9" style="2" customWidth="1"/>
     <col min="12" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
@@ -4243,7 +4342,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>27</v>
       </c>
@@ -4272,7 +4371,7 @@
         <v>29.641933869999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>28</v>
       </c>
@@ -4301,7 +4400,7 @@
         <v>23.544987089999999</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -4330,7 +4429,7 @@
         <v>85.862637930000005</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>30</v>
       </c>
@@ -4359,7 +4458,7 @@
         <v>42.502801900000001</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -4388,7 +4487,7 @@
         <v>35.940600340000003</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>32</v>
       </c>
@@ -4417,7 +4516,7 @@
         <v>59.933183769999999</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>33</v>
       </c>
@@ -4446,7 +4545,7 @@
         <v>106.8775864</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -4475,7 +4574,7 @@
         <v>22.948536409999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -4504,7 +4603,7 @@
         <v>24.503160529999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -4533,7 +4632,7 @@
         <v>42.124597010000002</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
@@ -4562,7 +4661,7 @@
         <v>14.355844429999999</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -4591,7 +4690,7 @@
         <v>23.90979467</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -4620,7 +4719,7 @@
         <v>18.821873790000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>40</v>
       </c>
@@ -4649,7 +4748,7 @@
         <v>16.075180710000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>41</v>
       </c>
@@ -4678,7 +4777,7 @@
         <v>14.668681100000001</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>42</v>
       </c>
@@ -4707,7 +4806,7 @@
         <v>17.20309584</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>43</v>
       </c>
@@ -4736,7 +4835,7 @@
         <v>16.054321989999998</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>44</v>
       </c>
@@ -4765,7 +4864,7 @@
         <v>12.0485469</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
@@ -4794,7 +4893,7 @@
         <v>30.745295809999998</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>46</v>
       </c>
@@ -4823,7 +4922,7 @@
         <v>24.29973292</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
README and Results update done by Samuel Whitby
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ground Segmentation\LiDAR-GS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC44711-61FD-4AAA-9CF2-6F59921EAC87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8C52FD-8300-4315-9CEA-E3EFAC7FCFF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="20832" windowHeight="16656" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17748" yWindow="0" windowWidth="23628" windowHeight="16656" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,13 @@
     <sheet name="GndNet" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="algorithm_name">README!$B$2</definedName>
-    <definedName name="cv_weight">README!$B$9</definedName>
-    <definedName name="iou_weight">README!$B$8</definedName>
-    <definedName name="pre_weight">README!$B$6</definedName>
-    <definedName name="rec_weight">README!$B$7</definedName>
-    <definedName name="system">README!$B$3</definedName>
+    <definedName name="algorithm_name">README!$C$10</definedName>
+    <definedName name="approach">README!$C$11</definedName>
+    <definedName name="cv_weight">README!$C$18</definedName>
+    <definedName name="iou_weight">README!$C$17</definedName>
+    <definedName name="pre_weight">README!$C$15</definedName>
+    <definedName name="rec_weight">README!$C$16</definedName>
+    <definedName name="system">README!$C$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,8 +48,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="81">
   <si>
     <t>Algorithm Name</t>
   </si>
@@ -194,9 +217,6 @@
     <t>Vld 64</t>
   </si>
   <si>
-    <t>Weights</t>
-  </si>
-  <si>
     <t>Precision</t>
   </si>
   <si>
@@ -213,13 +233,94 @@
   </si>
   <si>
     <t>Combined [%]</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>Ground Modelling</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>Please fill with algorithm name given in the evaluate_template.py</t>
+  </si>
+  <si>
+    <t>The sum of the weights must equal 1.</t>
+  </si>
+  <si>
+    <t>Welcome to the Results spreadsheet of the LiDAR-GS Benchmark. Please fill in the following boxes so that we can populate the performance scores for your algorithm. Once complete you can proceed to see how you compared to other algorithms in rural and rural environments and across different sensor types and positions. If you want to see your attribute results, please look for the sheet named after your algorithm.</t>
+  </si>
+  <si>
+    <t>What is the segmentation approach utilised (e.g. ground modelling, machine learning, etc.)</t>
+  </si>
+  <si>
+    <t>What is the processor used (CPU or GPU) and at what clock speed was it run?</t>
+  </si>
+  <si>
+    <t>LiDAR Ground Segmentation Benchmark Results</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Justification</t>
+  </si>
+  <si>
+    <t>Regarded as a safety concern as the algorithm failed to spot the ground points.</t>
+  </si>
+  <si>
+    <t>Although important, over-segmentation can be accounted for by traversability algorithms.</t>
+  </si>
+  <si>
+    <t>Arguably the most important metric in identifying safe algorithms.</t>
+  </si>
+  <si>
+    <t>This is an indicator of a consistent algorithm.</t>
+  </si>
+  <si>
+    <t>Frequent Issues</t>
+  </si>
+  <si>
+    <t>The cells arent populating</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>This is typically a naming issue, as the name input in this sheet must match the sheet name of the algorithm.</t>
+  </si>
+  <si>
+    <t>The leaderboard hasn’t changed</t>
+  </si>
+  <si>
+    <t>Unfortunately, this is a limitation of the spreadsheet. A self adjusting leaderboard will come in due course.</t>
+  </si>
+  <si>
+    <t>If you wish to submit the results of your algorithm or have any issues with the LiDAR-GS benchmark, feel free to contact me at: swhitby01@nmite.ac.uk</t>
+  </si>
+  <si>
+    <t>Contact Us</t>
+  </si>
+  <si>
+    <t>INPUT HERE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,44 +356,74 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="19">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -342,11 +473,120 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color auto="1"/>
@@ -354,52 +594,255 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -702,426 +1145,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:B10"/>
+  <dimension ref="B1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="1" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:4" ht="30" x14ac:dyDescent="0.5">
+      <c r="B2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13"/>
+    </row>
+    <row r="4" spans="2:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="17"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="13"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D10" s="26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C12" s="28" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D12" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="13"/>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="31" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C15" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="D15" s="34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="9">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C16" s="22">
+        <v>0.15</v>
+      </c>
+      <c r="D16" s="30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="32">
+        <v>0.4</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="9">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C18" s="22">
+        <v>0.2</v>
+      </c>
+      <c r="D18" s="30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="9">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="9">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" s="9">
-        <f>IF(OR(SUM(B6:B9)&gt;1, SUM(B6:B9)&lt;1), "Error!", SUM(B6:B9))</f>
+      <c r="C19" s="32">
+        <f>IF(OR(SUM(C15:C18)&gt;1, SUM(C15:C18)&lt;1), "Error!", SUM(C15:C18))</f>
         <v>1</v>
       </c>
+      <c r="D19" s="35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="37"/>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="39"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="37"/>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="13"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="13"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
+    </row>
+    <row r="27" spans="2:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="40"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="42"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="B26:D27"/>
+    <mergeCell ref="B4:D7"/>
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="41" width="8.69921875" style="1" customWidth="1"/>
-    <col min="42" max="16384" width="8.69921875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="2">
-        <f ca="1">IFERROR(E2*pre_weight+F2*rec_weight+G2*iou_weight+(100-H2)*cv_weight, "-")</f>
-        <v>90.950251101164923</v>
-      </c>
-      <c r="E2" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>85.301043171071314</v>
-      </c>
-      <c r="F2" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C2:C8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C9:C12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C13:C16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C17:C22")) * 0.25), "-")</f>
-        <v>96.525558037617117</v>
-      </c>
-      <c r="G2" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D2:D8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D9:D12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D13:D16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D17:D22")) * 0.25), "-")</f>
-        <v>88.1191344285333</v>
-      </c>
-      <c r="H2" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E2:E8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E9:E12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E13:E16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E17:E22")) * 0.25), "-")</f>
-        <v>0.50748584329402313</v>
-      </c>
-      <c r="I2" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F2:F8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F9:F12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F13:F16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F17:F22")) * 0.25), "-")</f>
-        <v>0.29917434715821811</v>
-      </c>
-      <c r="J2" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G2:G8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G9:G12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G13:G16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G17:G22")) * 0.25), "-")</f>
-        <v>3.8498463901689571E-3</v>
-      </c>
-      <c r="K2" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H2:H8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H9:H12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H13:H16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H17:H22")) * 0.25), "-")</f>
-        <v>0.16829877112135178</v>
-      </c>
-      <c r="L2" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>85.301043171071314</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="2">
-        <f ca="1">IFERROR(E3*pre_weight+F3*rec_weight+G3*iou_weight+(100-H3)*cv_weight, "-")</f>
-        <v>90.860776838740463</v>
-      </c>
-      <c r="E3" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>85.339570161553866</v>
-      </c>
-      <c r="F3" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!C2:C8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!C9:C12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!C13:C16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!C17:C22")) * 0.25), "-")</f>
-        <v>96.72901689687329</v>
-      </c>
-      <c r="G3" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!D2:D8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!D9:D12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!D13:D16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!D17:D22")) * 0.25), "-")</f>
-        <v>87.955077010562448</v>
-      </c>
-      <c r="H3" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!E2:E8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!E9:E12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!E13:E16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!E17:E22")) * 0.25), "-")</f>
-        <v>0.82749520201986226</v>
-      </c>
-      <c r="I3" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!F2:F8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!F9:F12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!F13:F16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!F17:F22")) * 0.25), "-")</f>
-        <v>0.51586981566820278</v>
-      </c>
-      <c r="J3" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!G2:G8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!G9:G12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!G13:G16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!G17:G22")) * 0.25), "-")</f>
-        <v>1.6474654377880125E-2</v>
-      </c>
-      <c r="K3" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!H2:H8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!H9:H12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!H13:H16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!H17:H22")) * 0.25), "-")</f>
-        <v>0.13277649769585251</v>
-      </c>
-      <c r="L3" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>85.339570161553866</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2">
-        <f ca="1">IFERROR(E4*pre_weight+F4*rec_weight+G4*iou_weight+(100-H4)*cv_weight, "-")</f>
-        <v>90.795555152982132</v>
-      </c>
-      <c r="E4" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>85.96215122430165</v>
-      </c>
-      <c r="F4" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C2:C8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C9:C12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C13:C16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C17:C22")) * 0.25), "-")</f>
-        <v>99.240129311587197</v>
-      </c>
-      <c r="G4" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D2:D8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D9:D12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D13:D16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D17:D22")) * 0.25), "-")</f>
-        <v>86.542859166400078</v>
-      </c>
-      <c r="H4" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E2:E8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E9:E12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E13:E16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E17:E22")) * 0.25), "-")</f>
-        <v>0.99072858195699953</v>
-      </c>
-      <c r="I4" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F2:F8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F9:F12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F13:F16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F17:F22")) * 0.25), "-")</f>
-        <v>17.01192396313364</v>
-      </c>
-      <c r="J4" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G2:G8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G9:G12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G13:G16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G17:G22")) * 0.25), "-")</f>
-        <v>-4.5122887864826539E-4</v>
-      </c>
-      <c r="K4" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H2:H8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H9:H12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H13:H16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H17:H22")) * 0.25), "-")</f>
-        <v>0.13008832565284179</v>
-      </c>
-      <c r="L4" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>85.96215122430165</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2">
-        <f ca="1">IFERROR(E5*pre_weight+F5*rec_weight+G5*iou_weight+(100-H5)*cv_weight, "-")</f>
-        <v>81.198195620805052</v>
-      </c>
-      <c r="E5" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>73.27891648961905</v>
-      </c>
-      <c r="F5" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!C2:C8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!C9:C12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!C13:C16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!C17:C22")) * 0.25), "-")</f>
-        <v>95.66850897241072</v>
-      </c>
-      <c r="G5" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!D2:D8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!D9:D12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!D13:D16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!D17:D22")) * 0.25), "-")</f>
-        <v>76.680753781154763</v>
-      </c>
-      <c r="H5" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!E2:E8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!E9:E12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!E13:E16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!E17:E22")) * 0.25), "-")</f>
-        <v>10.720556799616071</v>
-      </c>
-      <c r="I5" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!F2:F8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!F9:F12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!F13:F16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!F17:F22")) * 0.25), "-")</f>
-        <v>1.1057987711279762</v>
-      </c>
-      <c r="J5" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!G2:G8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!G9:G12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!G13:G16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!G17:G22")) * 0.25), "-")</f>
-        <v>-1.4967357943452383E-2</v>
-      </c>
-      <c r="K5" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!H2:H8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!H9:H12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!H13:H16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!H17:H22")) * 0.25), "-")</f>
-        <v>1.0584677419910715</v>
-      </c>
-      <c r="L5" s="2">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>73.27891648961905</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="str">
-        <f>algorithm_name</f>
-        <v>-</v>
-      </c>
-      <c r="D6" s="2" t="str">
-        <f ca="1">IFERROR(E6*0.3+F6*0.1+G6*0.4+(100-H6)*0.2, "-")</f>
-        <v>-</v>
-      </c>
-      <c r="E6" s="2" t="str">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="F6" s="2" t="str">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C2:C8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C9:C12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C13:C16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C17:C22")) * 0.25), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="G6" s="2" t="str">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D2:D8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D9:D12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D13:D16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D17:D22")) * 0.25), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="H6" s="2" t="str">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E2:E8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E9:E12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E13:E16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E17:E22")) * 0.25), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="I6" s="2" t="str">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F2:F8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F9:F12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F13:F16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F17:F22")) * 0.25), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="J6" s="2" t="str">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G2:G8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G9:G12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G13:G16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G17:G22")) * 0.25), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="K6" s="2" t="str">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H2:H8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H9:H12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H13:H16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H17:H22")) * 0.25), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="L6" s="2" t="str">
-        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B17:B22")) * 0.25), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="M6" s="1" t="str">
-        <f>system</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:N11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="1.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.8984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.59765625" style="1" bestFit="1" customWidth="1"/>
@@ -1137,565 +1417,923 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="76">
+        <v>1</v>
+      </c>
+      <c r="B2" s="70" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="77">
+        <f ca="1">IFERROR(F2*pre_weight+G2*rec_weight+H2*iou_weight+(100-I2)*cv_weight, "-")</f>
+        <v>90.950251101164923</v>
+      </c>
+      <c r="F2" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B17:B22")) * 0.25), "-")</f>
+        <v>85.301043171071314</v>
+      </c>
+      <c r="G2" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C2:C8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C9:C12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C13:C16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C17:C22")) * 0.25), "-")</f>
+        <v>96.525558037617117</v>
+      </c>
+      <c r="H2" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D2:D8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D9:D12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D13:D16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D17:D22")) * 0.25), "-")</f>
+        <v>88.1191344285333</v>
+      </c>
+      <c r="I2" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E2:E8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E9:E12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E13:E16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E17:E22")) * 0.25), "-")</f>
+        <v>0.50748584329402313</v>
+      </c>
+      <c r="J2" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F2:F8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F9:F12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F13:F16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F17:F22")) * 0.25), "-")</f>
+        <v>0.29917434715821811</v>
+      </c>
+      <c r="K2" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G2:G8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G9:G12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G13:G16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G17:G22")) * 0.25), "-")</f>
+        <v>3.8498463901689571E-3</v>
+      </c>
+      <c r="L2" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H2:H8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H9:H12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H13:H16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H17:H22")) * 0.25), "-")</f>
+        <v>0.16829877112135178</v>
+      </c>
+      <c r="M2" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B17:B22")) * 0.25), "-")</f>
+        <v>85.301043171071314</v>
+      </c>
+      <c r="N2" s="78" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="79">
+        <v>2</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="73" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="80">
+        <f ca="1">IFERROR(F3*pre_weight+G3*rec_weight+H3*iou_weight+(100-I3)*cv_weight, "-")</f>
+        <v>90.860776838740463</v>
+      </c>
+      <c r="F3" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B17:B22")) * 0.25), "-")</f>
+        <v>85.339570161553866</v>
+      </c>
+      <c r="G3" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!C2:C8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!C9:C12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!C13:C16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!C17:C22")) * 0.25), "-")</f>
+        <v>96.72901689687329</v>
+      </c>
+      <c r="H3" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!D2:D8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!D9:D12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!D13:D16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!D17:D22")) * 0.25), "-")</f>
+        <v>87.955077010562448</v>
+      </c>
+      <c r="I3" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!E2:E8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!E9:E12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!E13:E16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!E17:E22")) * 0.25), "-")</f>
+        <v>0.82749520201986226</v>
+      </c>
+      <c r="J3" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!F2:F8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!F9:F12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!F13:F16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!F17:F22")) * 0.25), "-")</f>
+        <v>0.51586981566820278</v>
+      </c>
+      <c r="K3" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!G2:G8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!G9:G12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!G13:G16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!G17:G22")) * 0.25), "-")</f>
+        <v>1.6474654377880125E-2</v>
+      </c>
+      <c r="L3" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!H2:H8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!H9:H12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!H13:H16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!H17:H22")) * 0.25), "-")</f>
+        <v>0.13277649769585251</v>
+      </c>
+      <c r="M3" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B3 &amp; "'!B17:B22")) * 0.25), "-")</f>
+        <v>85.339570161553866</v>
+      </c>
+      <c r="N3" s="81" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="76">
+        <v>3</v>
+      </c>
+      <c r="B4" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="71" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="77">
+        <f ca="1">IFERROR(F4*pre_weight+G4*rec_weight+H4*iou_weight+(100-I4)*cv_weight, "-")</f>
+        <v>90.795555152982132</v>
+      </c>
+      <c r="F4" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B17:B22")) * 0.25), "-")</f>
+        <v>85.96215122430165</v>
+      </c>
+      <c r="G4" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C2:C8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C9:C12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C13:C16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C17:C22")) * 0.25), "-")</f>
+        <v>99.240129311587197</v>
+      </c>
+      <c r="H4" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D2:D8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D9:D12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D13:D16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D17:D22")) * 0.25), "-")</f>
+        <v>86.542859166400078</v>
+      </c>
+      <c r="I4" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E2:E8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E9:E12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E13:E16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E17:E22")) * 0.25), "-")</f>
+        <v>0.99072858195699953</v>
+      </c>
+      <c r="J4" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F2:F8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F9:F12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F13:F16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F17:F22")) * 0.25), "-")</f>
+        <v>17.01192396313364</v>
+      </c>
+      <c r="K4" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G2:G8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G9:G12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G13:G16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G17:G22")) * 0.25), "-")</f>
+        <v>-4.5122887864826539E-4</v>
+      </c>
+      <c r="L4" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H2:H8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H9:H12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H13:H16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H17:H22")) * 0.25), "-")</f>
+        <v>0.13008832565284179</v>
+      </c>
+      <c r="M4" s="77">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B17:B22")) * 0.25), "-")</f>
+        <v>85.96215122430165</v>
+      </c>
+      <c r="N4" s="78" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="79">
+        <v>4</v>
+      </c>
+      <c r="B5" s="72" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="72" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="73" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="80">
+        <f ca="1">IFERROR(F5*pre_weight+G5*rec_weight+H5*iou_weight+(100-I5)*cv_weight, "-")</f>
+        <v>81.198195620805052</v>
+      </c>
+      <c r="F5" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B17:B22")) * 0.25), "-")</f>
+        <v>73.27891648961905</v>
+      </c>
+      <c r="G5" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!C2:C8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!C9:C12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!C13:C16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!C17:C22")) * 0.25), "-")</f>
+        <v>95.66850897241072</v>
+      </c>
+      <c r="H5" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!D2:D8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!D9:D12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!D13:D16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!D17:D22")) * 0.25), "-")</f>
+        <v>76.680753781154763</v>
+      </c>
+      <c r="I5" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!E2:E8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!E9:E12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!E13:E16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!E17:E22")) * 0.25), "-")</f>
+        <v>10.720556799616071</v>
+      </c>
+      <c r="J5" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!F2:F8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!F9:F12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!F13:F16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!F17:F22")) * 0.25), "-")</f>
+        <v>1.1057987711279762</v>
+      </c>
+      <c r="K5" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!G2:G8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!G9:G12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!G13:G16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!G17:G22")) * 0.25), "-")</f>
+        <v>-1.4967357943452383E-2</v>
+      </c>
+      <c r="L5" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!H2:H8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!H9:H12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!H13:H16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!H17:H22")) * 0.25), "-")</f>
+        <v>1.0584677419910715</v>
+      </c>
+      <c r="M5" s="80">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B5 &amp; "'!B17:B22")) * 0.25), "-")</f>
+        <v>73.27891648961905</v>
+      </c>
+      <c r="N5" s="81" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="82">
+        <v>5</v>
+      </c>
+      <c r="B6" s="74" t="str">
+        <f>algorithm_name</f>
+        <v>-</v>
+      </c>
+      <c r="C6" s="74" t="str" cm="1">
+        <f t="array" ref="C6">approach</f>
+        <v>-</v>
+      </c>
+      <c r="D6" s="75"/>
+      <c r="E6" s="83" t="str">
+        <f ca="1">IFERROR(F6*0.3+G6*0.1+H6*0.4+(100-I6)*0.2, "-")</f>
+        <v>-</v>
+      </c>
+      <c r="F6" s="83" t="str">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B17:B22")) * 0.25), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="G6" s="83" t="str">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C2:C8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C9:C12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C13:C16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C17:C22")) * 0.25), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="H6" s="83" t="str">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D2:D8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D9:D12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D13:D16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D17:D22")) * 0.25), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="I6" s="83" t="str">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E2:E8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E9:E12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E13:E16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E17:E22")) * 0.25), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="J6" s="83" t="str">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F2:F8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F9:F12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F13:F16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F17:F22")) * 0.25), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="K6" s="83" t="str">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G2:G8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G9:G12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G13:G16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G17:G22")) * 0.25), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="L6" s="83" t="str">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H2:H8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H9:H12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H13:H16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H17:H22")) * 0.25), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="M6" s="83" t="str">
+        <f ca="1">IFERROR(SUM(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B2:B8")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B9:B12")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B13:B16")) * 0.25, AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B17:B22")) * 0.25), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="N6" s="84" t="str">
+        <f>system</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D8" s="6"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{903D3E8C-B189-4ED9-B843-B766B3723587}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{07DBE870-C04B-468E-ACC7-CC69D9129DF6}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{B03B94E8-A2BF-4D76-9F29-980CEDA76208}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{767A8C7C-765A-4BFD-A769-8284693900AB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="42" width="8.69921875" style="1" customWidth="1"/>
+    <col min="43" max="16384" width="8.69921875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="45"/>
+      <c r="B1" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="48" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="61">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="85" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="63">
         <f ca="1">IFERROR(AVERAGE(E2:E3),"-")</f>
         <v>90.730086574554477</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="50">
         <f t="shared" ref="E2:E3" ca="1" si="0">IFERROR(F2*pre_weight+G2*rec_weight+H2*iou_weight+(100-I2)*cv_weight, "-")</f>
         <v>91.685283332814535</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B9:B12")), "-")</f>
         <v>87.132520116457528</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C9:C12")), "-")</f>
         <v>98.234119676471366</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D9:D12")), "-")</f>
         <v>88.464006043726442</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E9:E12")), "-")</f>
         <v>1.0928353263056589</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F9:F12")), "-")</f>
         <v>0.3564516129032258</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G9:G12")), "-")</f>
         <v>-8.0645161290322299E-4</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H9:H12")), "-")</f>
         <v>1.6129032258064516E-2</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!I9:I12")), "-")</f>
         <v>61.783431432306124</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="64" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="1" t="s">
+      <c r="A3" s="65"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="50">
         <f t="shared" ca="1" si="0"/>
         <v>89.774889816294419</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B2:B8")), "-")</f>
         <v>84.182073809950879</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C2:C8")), "-")</f>
         <v>98.631698999892038</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D2:D8")), "-")</f>
         <v>85.305095307992445</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E2:E8")), "-")</f>
         <v>0.93710804687043348</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F2:F8")), "-")</f>
         <v>0.20691244239631335</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G2:G8")), "-")</f>
         <v>-4.6082949308755598E-4</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H2:H8")), "-")</f>
         <v>7.3732718894009244E-2</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!I2:I8")), "-")</f>
         <v>94.301250454196307</v>
       </c>
-      <c r="N3" s="11"/>
+      <c r="N3" s="66"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="58">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="16">
-        <f t="shared" ref="C4:C11" ca="1" si="1">IFERROR(AVERAGE(E4:E5),"-")</f>
+      <c r="C4" s="59">
+        <f t="shared" ref="C4" ca="1" si="1">IFERROR(AVERAGE(E4:E5),"-")</f>
         <v>90.009220641129318</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="52">
         <f t="shared" ref="E4:E11" ca="1" si="2">IFERROR(F4*pre_weight+G4*rec_weight+H4*iou_weight+(100-I4)*cv_weight, "-")</f>
         <v>89.84015336241643</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B9:B12")), "-")</f>
         <v>84.481247839053438</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C9:C12")), "-")</f>
         <v>97.972552258545278</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D9:D12")), "-")</f>
         <v>85.984504763608982</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E9:E12")), "-")</f>
         <v>1.8492167078616293</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F9:F12")), "-")</f>
         <v>18.671774193548384</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G9:G12")), "-")</f>
         <v>8.8709677419356089E-3</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H9:H12")), "-")</f>
         <v>-1.6129032258064516E-2</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!I9:I12")), "-")</f>
         <v>32.745342136067734</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="60" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="1" t="s">
+      <c r="A5" s="58"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="52">
         <f t="shared" ca="1" si="2"/>
         <v>90.178287919842205</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B2:B8")), "-")</f>
         <v>85.273989895297632</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C2:C8")), "-")</f>
         <v>99.007174878695011</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D2:D8")), "-")</f>
         <v>86.078634345517045</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E2:E8")), "-")</f>
         <v>2.1136976199663691</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F2:F8")), "-")</f>
         <v>15.500921658986174</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G2:G8")), "-")</f>
         <v>5.9907834101382285E-3</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H2:H8")), "-")</f>
         <v>0.11981566820276499</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!I2:I8")), "-")</f>
         <v>32.550679183483389</v>
       </c>
-      <c r="N5" s="11"/>
+      <c r="N5" s="57"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="61">
         <v>3</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="16">
-        <f t="shared" ref="C6:C11" ca="1" si="3">IFERROR(AVERAGE(E6:E7),"-")</f>
+      <c r="C6" s="63">
+        <f t="shared" ref="C6" ca="1" si="3">IFERROR(AVERAGE(E6:E7),"-")</f>
         <v>89.91692889208457</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="50">
         <f t="shared" ca="1" si="2"/>
         <v>90.997344870744158</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B9:B12")), "-")</f>
         <v>86.140953438629055</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C9:C12")), "-")</f>
         <v>96.690725352351294</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D9:D12")), "-")</f>
         <v>88.400411526222427</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E9:E12")), "-")</f>
         <v>2.0083345112738544</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F9:F12")), "-")</f>
         <v>1.075</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G9:G12")), "-")</f>
         <v>4.8387096774193377E-3</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H9:H12")), "-")</f>
         <v>0.44354838709677424</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!I9:I12")), "-")</f>
         <v>97.730375137526224</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="64" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="1" t="s">
+      <c r="A7" s="61"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="50">
         <f t="shared" ca="1" si="2"/>
         <v>88.836512913424983</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B2:B8")), "-")</f>
         <v>81.316494372279379</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C2:C8")), "-")</f>
         <v>93.352206739636287</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D2:D8")), "-")</f>
         <v>86.912218921927007</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E2:E8")), "-")</f>
         <v>1.3016462968055944</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F2:F8")), "-")</f>
         <v>0.58847926267281114</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G2:G8")), "-")</f>
         <v>1.1059907834101343E-2</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H2:H8")), "-")</f>
         <v>8.7557603686635968E-2</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!I2:I8")), "-")</f>
         <v>92.681978262844083</v>
       </c>
-      <c r="N7" s="11"/>
+      <c r="N7" s="66"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="58">
         <v>4</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="16">
-        <f t="shared" ref="C8:C11" ca="1" si="4">IFERROR(AVERAGE(E8:E9),"-")</f>
+      <c r="C8" s="59">
+        <f t="shared" ref="C8" ca="1" si="4">IFERROR(AVERAGE(E8:E9),"-")</f>
         <v>69.576028661651776</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="89" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="52">
         <f t="shared" ca="1" si="2"/>
         <v>93.549025090524992</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!B9:B12")), "-")</f>
         <v>86.019075229999999</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!C9:C12")), "-")</f>
         <v>86.700224882500009</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!D9:D12")), "-")</f>
         <v>99.187658499999998</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!E9:E12")), "-")</f>
         <v>3.1792042467499999</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!F9:F12")), "-")</f>
         <v>0.78790322575000005</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!G9:G12")), "-")</f>
         <v>-8.0645162500000006E-3</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!H9:H12")), "-")</f>
         <v>0.32258064525000002</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!I9:I12")), "-")</f>
         <v>25.983034595000003</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="N8" s="60" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="1" t="s">
+      <c r="A9" s="58"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="52">
         <f t="shared" ca="1" si="2"/>
         <v>45.603032232778574</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!B2:B8")), "-")</f>
         <v>29.187782790142858</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!C2:C8")), "-")</f>
         <v>95.973811007142857</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!D2:D8")), "-")</f>
         <v>29.626548686285712</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!E2:E8")), "-")</f>
         <v>39.703022951714289</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!F2:F8")), "-")</f>
         <v>0.67695852542857149</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!G2:G8")), "-")</f>
         <v>-1.0138248857142857E-2</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!H2:H8")), "-")</f>
         <v>-0.83870967728571444</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!I2:I8")), "-")</f>
         <v>54.900533042857148</v>
       </c>
-      <c r="N9" s="11"/>
+      <c r="N9" s="57"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="61">
         <v>5</v>
       </c>
-      <c r="B10" s="12" t="str">
+      <c r="B10" s="85" t="str">
         <f>algorithm_name</f>
         <v>-</v>
       </c>
-      <c r="C10" s="16" t="str">
-        <f t="shared" ref="C10:C11" ca="1" si="5">IFERROR(AVERAGE(E10:E11),"-")</f>
+      <c r="C10" s="63" t="str">
+        <f t="shared" ref="C10" ca="1" si="5">IFERROR(AVERAGE(E10:E11),"-")</f>
         <v>-</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="2" t="str">
+      <c r="E10" s="50" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>-</v>
       </c>
-      <c r="F10" s="2" t="str">
+      <c r="F10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!B9:B12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="G10" s="2" t="str">
+      <c r="G10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!C9:C12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="H10" s="2" t="str">
+      <c r="H10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!D9:D12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="I10" s="2" t="str">
+      <c r="I10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!E9:E12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="J10" s="2" t="str">
+      <c r="J10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!F9:F12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="K10" s="2" t="str">
+      <c r="K10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!G9:G12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="L10" s="2" t="str">
+      <c r="L10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!H9:H12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="M10" s="2" t="str">
+      <c r="M10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!I9:I12")), "-")</f>
         <v>-</v>
       </c>
-      <c r="N10" s="12" t="str">
+      <c r="N10" s="64" t="str">
         <f>system</f>
         <v>-</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="1" t="s">
+    <row r="11" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="67"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="92" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="2" t="str">
+      <c r="E11" s="54" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>-</v>
       </c>
-      <c r="F11" s="2" t="str">
+      <c r="F11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!B2:B8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="G11" s="2" t="str">
+      <c r="G11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!C2:C8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="H11" s="2" t="str">
+      <c r="H11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!D2:D8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="I11" s="2" t="str">
+      <c r="I11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!E2:E8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="J11" s="2" t="str">
+      <c r="J11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!F2:F8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="K11" s="2" t="str">
+      <c r="K11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!G2:G8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="L11" s="2" t="str">
+      <c r="L11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!H2:H8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="M11" s="2" t="str">
+      <c r="M11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!I2:I8")), "-")</f>
         <v>-</v>
       </c>
-      <c r="N11" s="11"/>
+      <c r="N11" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="N2:N3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="N10:N11"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="N4:N5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="N4:N5"/>
     <mergeCell ref="N8:N9"/>
     <mergeCell ref="N6:N7"/>
-    <mergeCell ref="B8:B9"/>
     <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1707,7 +2345,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1715,7 +2353,7 @@
     <col min="1" max="1" width="1.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.796875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7.59765625" style="1" bestFit="1" customWidth="1"/>
@@ -1731,566 +2369,566 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="48" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="61">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="63">
         <f ca="1">IFERROR(AVERAGE(E2:E3),"-")</f>
         <v>92.820362579958342</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="50">
         <f t="shared" ref="E2:E9" ca="1" si="0">IFERROR(F2*pre_weight+G2*rec_weight+H2*iou_weight+(100-I2)*cv_weight, "-")</f>
         <v>99.304945170916682</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B17:B22")), "-")</f>
         <v>98.930684878333338</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C17:C22")), "-")</f>
         <v>100</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D17:D22")), "-")</f>
         <v>98.930684878333338</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E17:E22")), "-")</f>
         <v>0</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F17:F22")), "-")</f>
         <v>1.5833333333333333</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G17:G22")), "-")</f>
         <v>-1.6666666666666666E-2</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H17:H22")), "-")</f>
         <v>8</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!I17:I22")), "-")</f>
         <v>19.377807274999999</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="N2" s="64" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="1" t="s">
+      <c r="A3" s="65"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="50">
         <f t="shared" ca="1" si="0"/>
         <v>86.335779989000002</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!B13:B16")), "-")</f>
         <v>78.978123060000001</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!C13:C16")), "-")</f>
         <v>100</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!D13:D16")), "-")</f>
         <v>78.978123060000001</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!E13:E16")), "-")</f>
         <v>0</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!F13:F16")), "-")</f>
         <v>1.375</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!G13:G16")), "-")</f>
         <v>-2.5000000000000001E-2</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!H13:H16")), "-")</f>
         <v>-3.25</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M3" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B2 &amp; "'!I13:I16")), "-")</f>
         <v>18.368882567500002</v>
       </c>
-      <c r="N3" s="11"/>
+      <c r="N3" s="66"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="58">
         <v>2</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="16">
-        <f t="shared" ref="C4:C11" ca="1" si="1">IFERROR(AVERAGE(E4:E5),"-")</f>
+      <c r="C4" s="59">
+        <f t="shared" ref="C4" ca="1" si="1">IFERROR(AVERAGE(E4:E5),"-")</f>
         <v>91.804624785396385</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="52">
         <f t="shared" ca="1" si="0"/>
         <v>93.412023331820023</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B17:B22")), "-")</f>
         <v>89.163734620541391</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C17:C22")), "-")</f>
         <v>97.628049265160499</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D17:D22")), "-")</f>
         <v>91.19220571727648</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E17:E22")), "-")</f>
         <v>0</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F17:F22")), "-")</f>
         <v>0.19999999999999998</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G17:G22")), "-")</f>
         <v>0</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H17:H22")), "-")</f>
         <v>-0.50000000000000011</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!I17:I22")), "-")</f>
         <v>146.35557969909368</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="N4" s="60" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="1" t="s">
+      <c r="A5" s="55"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="52">
         <f t="shared" ca="1" si="0"/>
         <v>90.197226238972732</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!B13:B16")), "-")</f>
         <v>84.737098214765638</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!C13:C16")), "-")</f>
         <v>99.245086230345109</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!D13:D16")), "-")</f>
         <v>85.315471876823878</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!E13:E16")), "-")</f>
         <v>0</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!F13:F16")), "-")</f>
         <v>0.19999999999999998</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!G13:G16")), "-")</f>
         <v>4.9999999999999822E-2</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!H13:H16")), "-")</f>
         <v>0.5</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B4 &amp; "'!I13:I16")), "-")</f>
         <v>96.245946276680598</v>
       </c>
-      <c r="N5" s="11"/>
+      <c r="N5" s="57"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="61">
         <v>3</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="85" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="16">
-        <f t="shared" ref="C6:C11" ca="1" si="2">IFERROR(AVERAGE(E6:E7),"-")</f>
+      <c r="C6" s="63">
+        <f t="shared" ref="C6" ca="1" si="2">IFERROR(AVERAGE(E6:E7),"-")</f>
         <v>91.581889664834932</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="50">
         <f t="shared" ca="1" si="0"/>
         <v>93.877317485517025</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B17:B22")), "-")</f>
         <v>90.577744542562314</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C17:C22")), "-")</f>
         <v>99.989442673142193</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D17:D22")), "-")</f>
         <v>90.586162372262791</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E17:E22")), "-")</f>
         <v>0</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F17:F22")), "-")</f>
         <v>15.4</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G17:G22")), "-")</f>
         <v>-1.6666666666666899E-2</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H17:H22")), "-")</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!I17:I22")), "-")</f>
         <v>48.746001630501063</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="64" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="1" t="s">
+      <c r="A7" s="65"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="50">
         <f t="shared" ca="1" si="0"/>
         <v>89.286461844152839</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!B13:B16")), "-")</f>
         <v>83.515622620293229</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!C13:C16")), "-")</f>
         <v>99.991347435966304</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!D13:D16")), "-")</f>
         <v>83.522135184211464</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!E13:E16")), "-")</f>
         <v>0</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!F13:F16")), "-")</f>
         <v>18.475000000000001</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!G13:G16")), "-")</f>
         <v>0</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!H13:H16")), "-")</f>
         <v>0.25</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="50">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B6 &amp; "'!I13:I16")), "-")</f>
         <v>29.583004715014212</v>
       </c>
-      <c r="N7" s="11"/>
+      <c r="N7" s="66"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="58">
         <v>4</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="16">
-        <f t="shared" ref="C8:C11" ca="1" si="3">IFERROR(AVERAGE(E8:E9),"-")</f>
+      <c r="C8" s="59">
+        <f t="shared" ref="C8" ca="1" si="3">IFERROR(AVERAGE(E8:E9),"-")</f>
         <v>91.170415627775355</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="52">
         <f t="shared" ca="1" si="0"/>
         <v>92.616228914278651</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!B17:B22")), "-")</f>
         <v>88.111774280571254</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!C17:C22")), "-")</f>
         <v>97.877081461267494</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!D17:D22")), "-")</f>
         <v>89.766807812364291</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!E17:E22")), "-")</f>
         <v>0</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!F17:F22")), "-")</f>
         <v>0.38333333333333336</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!G17:G22")), "-")</f>
         <v>1.6666666666666607E-2</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!H17:H22")), "-")</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!I17:I22")), "-")</f>
         <v>108.2016928782039</v>
       </c>
-      <c r="N8" s="12" t="s">
+      <c r="N8" s="60" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="1" t="s">
+      <c r="A9" s="55"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="52">
         <f t="shared" ca="1" si="0"/>
         <v>89.72460234127206</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!B13:B16")), "-")</f>
         <v>81.77780447730558</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!C13:C16")), "-")</f>
         <v>91.359332012837541</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!D13:D16")), "-")</f>
         <v>88.940628550050064</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!E13:E16")), "-")</f>
         <v>0</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!F13:F16")), "-")</f>
         <v>0.25</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!G13:G16")), "-")</f>
         <v>0</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!H13:H16")), "-")</f>
         <v>0.25</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="52">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B8 &amp; "'!I13:I16")), "-")</f>
         <v>62.89510744849359</v>
       </c>
-      <c r="N9" s="11"/>
+      <c r="N9" s="57"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="61">
         <v>5</v>
       </c>
-      <c r="B10" s="12" t="str">
+      <c r="B10" s="85" t="str">
         <f>algorithm_name</f>
         <v>-</v>
       </c>
-      <c r="C10" s="16" t="str">
-        <f t="shared" ref="C10:C11" ca="1" si="4">IFERROR(AVERAGE(E10:E11),"-")</f>
+      <c r="C10" s="63" t="str">
+        <f t="shared" ref="C10" ca="1" si="4">IFERROR(AVERAGE(E10:E11),"-")</f>
         <v>-</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="2" t="str">
+      <c r="E10" s="50" t="str">
         <f t="shared" ref="E10:E11" ca="1" si="5">IFERROR(F10*pre_weight+G10*rec_weight+H10*iou_weight+(100-I10)*cv_weight, "-")</f>
         <v>-</v>
       </c>
-      <c r="F10" s="2" t="str">
+      <c r="F10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!B17:B22")), "-")</f>
         <v>-</v>
       </c>
-      <c r="G10" s="2" t="str">
+      <c r="G10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!C17:C22")), "-")</f>
         <v>-</v>
       </c>
-      <c r="H10" s="2" t="str">
+      <c r="H10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!D17:D22")), "-")</f>
         <v>-</v>
       </c>
-      <c r="I10" s="2" t="str">
+      <c r="I10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!E17:E22")), "-")</f>
         <v>-</v>
       </c>
-      <c r="J10" s="2" t="str">
+      <c r="J10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!F17:F22")), "-")</f>
         <v>-</v>
       </c>
-      <c r="K10" s="2" t="str">
+      <c r="K10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!G17:G22")), "-")</f>
         <v>-</v>
       </c>
-      <c r="L10" s="2" t="str">
+      <c r="L10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!H17:H22")), "-")</f>
         <v>-</v>
       </c>
-      <c r="M10" s="2" t="str">
+      <c r="M10" s="50" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!I17:I22")), "-")</f>
         <v>-</v>
       </c>
-      <c r="N10" s="12" t="str">
+      <c r="N10" s="64" t="str">
         <f>system</f>
         <v>-</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="1" t="s">
+    <row r="11" spans="1:14" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="67"/>
+      <c r="B11" s="91"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="2" t="str">
+      <c r="E11" s="54" t="str">
         <f t="shared" ca="1" si="5"/>
         <v>-</v>
       </c>
-      <c r="F11" s="2" t="str">
+      <c r="F11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!B13:B16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="G11" s="2" t="str">
+      <c r="G11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!C13:C16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="H11" s="2" t="str">
+      <c r="H11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!D13:D16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="I11" s="2" t="str">
+      <c r="I11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!E13:E16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="J11" s="2" t="str">
+      <c r="J11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!F13:F16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="K11" s="2" t="str">
+      <c r="K11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!G13:G16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="L11" s="2" t="str">
+      <c r="L11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!H13:H16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="M11" s="2" t="str">
+      <c r="M11" s="54" t="str">
         <f ca="1">IFERROR(AVERAGE(INDIRECT("'" &amp; $B10 &amp; "'!I13:I16")), "-")</f>
         <v>-</v>
       </c>
-      <c r="N11" s="11"/>
+      <c r="N11" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="N10:N11"/>
     <mergeCell ref="A8:A9"/>
-    <mergeCell ref="N8:N9"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="N8:N9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2319,31 +2957,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2966,7 +3604,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2984,31 +3622,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3649,31 +4287,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4314,31 +4952,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="5" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>